<commit_message>
fixed excel files for 20 bus grid
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_1_bus.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_1_bus.xlsx
@@ -8706,16 +8706,16 @@
         <v>0.9987117638702924</v>
       </c>
       <c r="O2">
-        <v>0.1709787174874783</v>
+        <v>0.1709787174874782</v>
       </c>
       <c r="P2">
-        <v>0.9122454452052585</v>
+        <v>0.9122454452052583</v>
       </c>
       <c r="Q2">
-        <v>4.230599833991775</v>
+        <v>4.230599833991791</v>
       </c>
       <c r="R2">
-        <v>-120.4793123293236</v>
+        <v>-120.4793123293238</v>
       </c>
       <c r="S2">
         <v>175.3675689136774</v>
@@ -8729,49 +8729,49 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2.174063364664713</v>
+        <v>2.174063364664714</v>
       </c>
       <c r="D3">
-        <v>2.174063364664713</v>
+        <v>2.174063364664714</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>25.10392137648951</v>
+        <v>25.10392137648953</v>
       </c>
       <c r="G3">
-        <v>25.10392137648951</v>
+        <v>25.10392137648953</v>
       </c>
       <c r="H3">
-        <v>4.185910274912399</v>
+        <v>4.185910274912402</v>
       </c>
       <c r="I3">
-        <v>5.870495034006284</v>
+        <v>5.870495034006279</v>
       </c>
       <c r="J3">
-        <v>0.9578163680532483</v>
+        <v>0.957816368053249</v>
       </c>
       <c r="K3">
-        <v>4.968163485641733</v>
+        <v>4.968163485641724</v>
       </c>
       <c r="L3">
-        <v>0.9578163680261339</v>
+        <v>0.957816368026136</v>
       </c>
       <c r="M3">
-        <v>4.968163485594578</v>
+        <v>4.968163485594566</v>
       </c>
       <c r="N3">
-        <v>0.9526279648092827</v>
+        <v>0.9526279648092829</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.952627964809529</v>
+        <v>0.9526279648095289</v>
       </c>
       <c r="Q3">
-        <v>-4.852401742958505E-13</v>
+        <v>-4.690603644824303E-13</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8821,22 +8821,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279648003588</v>
+        <v>0.9526279648003591</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279648184529</v>
+        <v>0.9526279648184528</v>
       </c>
       <c r="Q4">
-        <v>4.725556934297731E-10</v>
+        <v>4.725740290213336E-10</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.9999999995189</v>
+        <v>179.999999999519</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -8886,16 +8886,16 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279648184529</v>
+        <v>0.9526279648184526</v>
       </c>
       <c r="Q5">
-        <v>4.725561278548703E-10</v>
+        <v>4.725761522894142E-10</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999995189</v>
+        <v>179.999999999519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>